<commit_message>
Add new columns (login password)
</commit_message>
<xml_diff>
--- a/PlanBD.xlsx
+++ b/PlanBD.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">Макет БД</t>
   </si>
@@ -33,6 +33,12 @@
     <t xml:space="preserve">FIO (TEXT)</t>
   </si>
   <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
     <t xml:space="preserve">filial (TEXT)</t>
   </si>
   <si>
@@ -54,25 +60,43 @@
     <t xml:space="preserve">Иванов Иван Иванович</t>
   </si>
   <si>
+    <t>mylogin1</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
     <t>Филиал1</t>
   </si>
   <si>
     <t>Сотрудник2</t>
   </si>
   <si>
+    <t>mylogin2</t>
+  </si>
+  <si>
     <t>Филиал2</t>
   </si>
   <si>
     <t>Сотрудник3</t>
   </si>
   <si>
+    <t>mylogin3</t>
+  </si>
+  <si>
     <t>Филиал3</t>
   </si>
   <si>
     <t>Сотрудник4</t>
   </si>
   <si>
+    <t>mylogin4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Директоров Андрей Викторович</t>
+  </si>
+  <si>
+    <t>mylogin5</t>
   </si>
 </sst>
 </file>
@@ -138,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -154,13 +178,12 @@
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,12 +701,12 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="31.7109375"/>
-    <col customWidth="1" min="2" max="3" width="40.140625"/>
-    <col customWidth="1" min="4" max="5" width="18.140625"/>
-    <col customWidth="1" min="7" max="7" width="35.57421875"/>
-    <col customWidth="1" min="8" max="8" width="27.8515625"/>
-    <col customWidth="1" min="9" max="9" width="24.8515625"/>
-    <col customWidth="1" min="10" max="10" width="26.421875"/>
+    <col customWidth="1" min="2" max="5" width="40.140625"/>
+    <col customWidth="1" min="6" max="7" width="18.140625"/>
+    <col customWidth="1" min="9" max="9" width="35.57421875"/>
+    <col customWidth="1" min="10" max="10" width="27.8515625"/>
+    <col customWidth="1" min="11" max="11" width="24.8515625"/>
+    <col customWidth="1" min="12" max="12" width="26.421875"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.75">
@@ -699,6 +722,8 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" ht="17.25">
       <c r="A2" s="3" t="s">
@@ -708,17 +733,19 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" ht="17.25">
       <c r="A3" s="6" t="s">
@@ -733,10 +760,10 @@
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -745,318 +772,392 @@
       <c r="J3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="K3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
     </row>
     <row r="4" ht="17.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6">
         <v>0</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6">
-        <v>1</v>
       </c>
       <c r="I4" s="6">
         <v>1</v>
       </c>
       <c r="J4" s="6">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1</v>
+      </c>
+      <c r="L4" s="6">
         <v>30000</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
     </row>
     <row r="5" ht="17.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D5" s="6">
+        <v>1111</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="6">
         <v>0</v>
       </c>
-      <c r="G5" s="6">
+      <c r="I5" s="6">
         <v>2</v>
       </c>
-      <c r="H5" s="6">
+      <c r="J5" s="6">
         <v>1</v>
       </c>
-      <c r="I5" s="6">
+      <c r="K5" s="6">
         <v>3</v>
       </c>
-      <c r="J5" s="6">
+      <c r="L5" s="6">
         <v>30000</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" ht="17.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D6" s="6">
+        <v>2222</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="6">
         <v>0</v>
       </c>
-      <c r="G6" s="6">
+      <c r="I6" s="6">
         <v>3</v>
       </c>
-      <c r="H6" s="6">
+      <c r="J6" s="6">
         <v>2</v>
       </c>
-      <c r="I6" s="6">
+      <c r="K6" s="6">
         <v>1</v>
       </c>
-      <c r="J6" s="6">
+      <c r="L6" s="6">
         <v>20000</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
     </row>
     <row r="7" ht="17.25">
       <c r="A7" s="6">
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D7" s="6">
+        <v>3333</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="6">
         <v>0</v>
       </c>
-      <c r="G7" s="6">
+      <c r="I7" s="6">
         <v>4</v>
       </c>
-      <c r="H7" s="6">
+      <c r="J7" s="6">
         <v>2</v>
       </c>
-      <c r="I7" s="6">
+      <c r="K7" s="6">
         <v>2</v>
       </c>
-      <c r="J7" s="6">
+      <c r="L7" s="6">
         <v>10000</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
     </row>
     <row r="8" ht="17.25">
       <c r="A8" s="6">
         <v>5</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D8" s="6">
+        <v>4444</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="6">
         <v>1</v>
       </c>
-      <c r="G8" s="6">
+      <c r="I8" s="6">
         <v>5</v>
       </c>
-      <c r="H8" s="6">
+      <c r="J8" s="6">
         <v>2</v>
       </c>
-      <c r="I8" s="6">
+      <c r="K8" s="6">
         <v>3</v>
       </c>
-      <c r="J8" s="6">
+      <c r="L8" s="6">
         <v>10000</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
     </row>
     <row r="9" ht="17.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
     </row>
     <row r="10" ht="17.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" ht="17.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" ht="17.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13" ht="17.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" ht="17.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" ht="17.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" ht="17.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" ht="17.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" ht="17.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" ht="17.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20" ht="17.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" ht="17.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" ht="17.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" ht="17.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" ht="17.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
     </row>
     <row r="25" ht="17.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="9"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" ht="17.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="9"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" ht="17.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="9"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="I2:L2"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>